<commit_message>
Updated todays working hours
</commit_message>
<xml_diff>
--- a/2018+Arbeitszeiterfassung+Michael+Pl%c3%bcss.xlsx
+++ b/2018+Arbeitszeiterfassung+Michael+Pl%c3%bcss.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Dez!$A$1:$M$47</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Dez!$A$1:$M$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Dez!$A$1:$M$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -46,17 +47,8 @@
 Stunden</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Bemerkungen
+    <t xml:space="preserve">Bemerkungen
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Sa</t>
@@ -560,7 +552,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="131">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -793,10 +785,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -999,10 +987,6 @@
     </xf>
     <xf numFmtId="169" fontId="7" fillId="2" borderId="39" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1219,20 +1203,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.64285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.51020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.39795918367347"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="57.3724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="56.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10485,7 +10469,7 @@
       <c r="AMI9" s="0"/>
       <c r="AMJ9" s="0"/>
     </row>
-    <row r="10" s="58" customFormat="true" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="n">
         <v>1</v>
       </c>
@@ -10504,7 +10488,7 @@
       <c r="L10" s="56"/>
       <c r="M10" s="57"/>
     </row>
-    <row r="11" s="58" customFormat="true" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="n">
         <v>2</v>
       </c>
@@ -10524,23 +10508,23 @@
       <c r="M11" s="57"/>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="59" t="n">
+      <c r="A12" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="64"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="63"/>
       <c r="N12" s="0"/>
       <c r="O12" s="0"/>
       <c r="P12" s="0"/>
@@ -11554,23 +11538,23 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="59" t="n">
+      <c r="A13" s="58" t="n">
         <v>4</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="64"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="63"/>
       <c r="N13" s="0"/>
       <c r="O13" s="0"/>
       <c r="P13" s="0"/>
@@ -12584,23 +12568,23 @@
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="59" t="n">
+      <c r="A14" s="58" t="n">
         <v>5</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="65"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="68"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="67"/>
       <c r="N14" s="0"/>
       <c r="O14" s="0"/>
       <c r="P14" s="0"/>
@@ -13614,25 +13598,25 @@
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="59" t="n">
+      <c r="A15" s="58" t="n">
         <v>6</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="65" t="n">
+      <c r="C15" s="64" t="n">
         <v>3.5</v>
       </c>
-      <c r="D15" s="66"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="69" t="s">
+      <c r="D15" s="65"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="68" t="s">
         <v>13</v>
       </c>
       <c r="N15" s="0"/>
@@ -14648,23 +14632,25 @@
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="59" t="n">
+      <c r="A16" s="58" t="n">
         <v>7</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="69"/>
+      <c r="C16" s="64" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D16" s="65"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="68"/>
       <c r="N16" s="0"/>
       <c r="O16" s="0"/>
       <c r="P16" s="0"/>
@@ -15694,7 +15680,7 @@
       <c r="J17" s="55"/>
       <c r="K17" s="54"/>
       <c r="L17" s="56"/>
-      <c r="M17" s="70"/>
+      <c r="M17" s="69"/>
       <c r="N17" s="0"/>
       <c r="O17" s="0"/>
       <c r="P17" s="0"/>
@@ -16724,7 +16710,7 @@
       <c r="J18" s="55"/>
       <c r="K18" s="54"/>
       <c r="L18" s="56"/>
-      <c r="M18" s="70"/>
+      <c r="M18" s="69"/>
       <c r="N18" s="0"/>
       <c r="O18" s="0"/>
       <c r="P18" s="0"/>
@@ -17738,23 +17724,23 @@
       <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="59" t="n">
+      <c r="A19" s="58" t="n">
         <v>10</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="63"/>
-      <c r="M19" s="71"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="70"/>
       <c r="N19" s="0"/>
       <c r="O19" s="0"/>
       <c r="P19" s="0"/>
@@ -18768,23 +18754,23 @@
       <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="59" t="n">
+      <c r="A20" s="58" t="n">
         <v>11</v>
       </c>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="63"/>
-      <c r="M20" s="71"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="70"/>
       <c r="N20" s="0"/>
       <c r="O20" s="0"/>
       <c r="P20" s="0"/>
@@ -19798,23 +19784,23 @@
       <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="59" t="n">
+      <c r="A21" s="58" t="n">
         <v>12</v>
       </c>
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="69"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="68"/>
       <c r="N21" s="0"/>
       <c r="O21" s="0"/>
       <c r="P21" s="0"/>
@@ -20828,23 +20814,23 @@
       <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="59" t="n">
+      <c r="A22" s="58" t="n">
         <v>13</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="67"/>
-      <c r="M22" s="69"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="68"/>
       <c r="N22" s="0"/>
       <c r="O22" s="0"/>
       <c r="P22" s="0"/>
@@ -21858,23 +21844,23 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="59" t="n">
+      <c r="A23" s="58" t="n">
         <v>14</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="67"/>
-      <c r="M23" s="69"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="68"/>
       <c r="N23" s="0"/>
       <c r="O23" s="0"/>
       <c r="P23" s="0"/>
@@ -22904,7 +22890,7 @@
       <c r="J24" s="55"/>
       <c r="K24" s="54"/>
       <c r="L24" s="56"/>
-      <c r="M24" s="70"/>
+      <c r="M24" s="69"/>
       <c r="N24" s="0"/>
       <c r="O24" s="0"/>
       <c r="P24" s="0"/>
@@ -23934,7 +23920,7 @@
       <c r="J25" s="55"/>
       <c r="K25" s="54"/>
       <c r="L25" s="56"/>
-      <c r="M25" s="70"/>
+      <c r="M25" s="69"/>
       <c r="N25" s="0"/>
       <c r="O25" s="0"/>
       <c r="P25" s="0"/>
@@ -24948,23 +24934,23 @@
       <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="59" t="n">
+      <c r="A26" s="58" t="n">
         <v>17</v>
       </c>
-      <c r="B26" s="60" t="s">
+      <c r="B26" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="63"/>
-      <c r="M26" s="71"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="70"/>
       <c r="N26" s="0"/>
       <c r="O26" s="0"/>
       <c r="P26" s="0"/>
@@ -25978,23 +25964,23 @@
       <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="59" t="n">
+      <c r="A27" s="58" t="n">
         <v>18</v>
       </c>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="71"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="70"/>
       <c r="N27" s="0"/>
       <c r="O27" s="0"/>
       <c r="P27" s="0"/>
@@ -27008,23 +26994,23 @@
       <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="59" t="n">
+      <c r="A28" s="58" t="n">
         <v>19</v>
       </c>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="69"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="68"/>
       <c r="N28" s="0"/>
       <c r="O28" s="0"/>
       <c r="P28" s="0"/>
@@ -28038,23 +28024,23 @@
       <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="59" t="n">
+      <c r="A29" s="58" t="n">
         <v>20</v>
       </c>
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="65"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="67"/>
-      <c r="M29" s="69"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="68"/>
       <c r="N29" s="0"/>
       <c r="O29" s="0"/>
       <c r="P29" s="0"/>
@@ -29068,23 +29054,23 @@
       <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="59" t="n">
+      <c r="A30" s="58" t="n">
         <v>21</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="67"/>
-      <c r="M30" s="69"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="66"/>
+      <c r="M30" s="68"/>
       <c r="N30" s="0"/>
       <c r="O30" s="0"/>
       <c r="P30" s="0"/>
@@ -30114,7 +30100,7 @@
       <c r="J31" s="55"/>
       <c r="K31" s="54"/>
       <c r="L31" s="56"/>
-      <c r="M31" s="70"/>
+      <c r="M31" s="69"/>
       <c r="N31" s="0"/>
       <c r="O31" s="0"/>
       <c r="P31" s="0"/>
@@ -31144,7 +31130,7 @@
       <c r="J32" s="55"/>
       <c r="K32" s="54"/>
       <c r="L32" s="56"/>
-      <c r="M32" s="70"/>
+      <c r="M32" s="69"/>
       <c r="N32" s="0"/>
       <c r="O32" s="0"/>
       <c r="P32" s="0"/>
@@ -32158,26 +32144,26 @@
       <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="59" t="n">
+      <c r="A33" s="58" t="n">
         <v>24</v>
       </c>
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="63"/>
-      <c r="M33" s="71" t="s">
+      <c r="C33" s="60"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="N33" s="72" t="s">
+      <c r="N33" s="71" t="s">
         <v>16</v>
       </c>
       <c r="O33" s="0"/>
@@ -33198,17 +33184,17 @@
       <c r="B34" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="75"/>
-      <c r="M34" s="76" t="s">
+      <c r="C34" s="72"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="75" t="s">
         <v>17</v>
       </c>
       <c r="N34" s="0"/>
@@ -34223,7 +34209,7 @@
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" s="77" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="76" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="52" t="n">
         <v>26</v>
       </c>
@@ -34240,47 +34226,47 @@
       <c r="J35" s="55"/>
       <c r="K35" s="54"/>
       <c r="L35" s="56"/>
-      <c r="M35" s="70" t="s">
+      <c r="M35" s="69" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" s="58" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="59" t="n">
+    <row r="36" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="58" t="n">
         <v>27</v>
       </c>
-      <c r="B36" s="60" t="s">
+      <c r="B36" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="65"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="69"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="68"/>
     </row>
-    <row r="37" s="58" customFormat="true" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="59" t="n">
+    <row r="37" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="58" t="n">
         <v>28</v>
       </c>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="65"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="65"/>
-      <c r="L37" s="67"/>
-      <c r="M37" s="69"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="65"/>
+      <c r="K37" s="64"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="68"/>
     </row>
     <row r="38" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="52" t="n">
@@ -34299,7 +34285,7 @@
       <c r="J38" s="55"/>
       <c r="K38" s="54"/>
       <c r="L38" s="56"/>
-      <c r="M38" s="70"/>
+      <c r="M38" s="69"/>
       <c r="N38" s="0"/>
       <c r="O38" s="0"/>
       <c r="P38" s="0"/>
@@ -35329,7 +35315,7 @@
       <c r="J39" s="55"/>
       <c r="K39" s="54"/>
       <c r="L39" s="56"/>
-      <c r="M39" s="70"/>
+      <c r="M39" s="69"/>
       <c r="N39" s="0"/>
       <c r="O39" s="0"/>
       <c r="P39" s="0"/>
@@ -36343,23 +36329,23 @@
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="78" t="n">
+      <c r="A40" s="77" t="n">
         <v>31</v>
       </c>
-      <c r="B40" s="60" t="s">
+      <c r="B40" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="79"/>
-      <c r="D40" s="66"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="80"/>
-      <c r="I40" s="79"/>
-      <c r="J40" s="80"/>
-      <c r="K40" s="79"/>
-      <c r="L40" s="81"/>
-      <c r="M40" s="82" t="s">
+      <c r="C40" s="78"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="79"/>
+      <c r="I40" s="78"/>
+      <c r="J40" s="79"/>
+      <c r="K40" s="78"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="81" t="s">
         <v>19</v>
       </c>
       <c r="N40" s="0"/>
@@ -37375,48 +37361,48 @@
       <c r="AMJ40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="83" t="s">
+      <c r="A41" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="83"/>
-      <c r="C41" s="84" t="n">
+      <c r="B41" s="82"/>
+      <c r="C41" s="83" t="n">
         <f aca="false">SUM(C10:C40)</f>
-        <v>3.5</v>
+        <v>6</v>
       </c>
-      <c r="D41" s="85"/>
-      <c r="E41" s="86" t="n">
+      <c r="D41" s="84"/>
+      <c r="E41" s="85" t="n">
         <f aca="false">SUM(E10:E40)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="85" t="n">
+      <c r="F41" s="84" t="n">
         <f aca="false">SUM(F10:F40)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="86" t="n">
+      <c r="G41" s="85" t="n">
         <f aca="false">SUM(G10:G40)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="85" t="n">
+      <c r="H41" s="84" t="n">
         <f aca="false">SUM(H10:H40)</f>
         <v>0</v>
       </c>
-      <c r="I41" s="86" t="n">
+      <c r="I41" s="85" t="n">
         <f aca="false">SUM(I10:I40)</f>
         <v>0</v>
       </c>
-      <c r="J41" s="85" t="n">
+      <c r="J41" s="84" t="n">
         <f aca="false">SUM(J10:J40)</f>
         <v>0</v>
       </c>
-      <c r="K41" s="86" t="n">
+      <c r="K41" s="85" t="n">
         <f aca="false">SUM(K10:K40)</f>
         <v>0</v>
       </c>
-      <c r="L41" s="87" t="n">
+      <c r="L41" s="86" t="n">
         <f aca="false">SUM(L10:L40)</f>
         <v>0</v>
       </c>
-      <c r="M41" s="88"/>
+      <c r="M41" s="87"/>
       <c r="N41" s="0"/>
       <c r="O41" s="0"/>
       <c r="P41" s="0"/>
@@ -38430,23 +38416,23 @@
       <c r="AMJ41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="89" t="s">
+      <c r="A42" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="89"/>
-      <c r="C42" s="90" t="n">
+      <c r="B42" s="88"/>
+      <c r="C42" s="89" t="n">
         <v>40</v>
       </c>
-      <c r="D42" s="91"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="92"/>
-      <c r="H42" s="93"/>
-      <c r="I42" s="94"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="96"/>
-      <c r="L42" s="97"/>
-      <c r="M42" s="98"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="92"/>
+      <c r="I42" s="93"/>
+      <c r="J42" s="94"/>
+      <c r="K42" s="95"/>
+      <c r="L42" s="96"/>
+      <c r="M42" s="97"/>
       <c r="N42" s="0"/>
       <c r="O42" s="0"/>
       <c r="P42" s="0"/>
@@ -39459,104 +39445,104 @@
       <c r="AMI42" s="0"/>
       <c r="AMJ42" s="0"/>
     </row>
-    <row r="43" s="110" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="99" t="s">
+    <row r="43" s="71" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="99"/>
-      <c r="C43" s="100" t="n">
+      <c r="B43" s="98"/>
+      <c r="C43" s="99" t="n">
         <f aca="false">C41*C42</f>
-        <v>140</v>
+        <v>240</v>
       </c>
-      <c r="D43" s="101"/>
-      <c r="E43" s="102"/>
-      <c r="F43" s="103"/>
-      <c r="G43" s="103"/>
-      <c r="H43" s="104"/>
-      <c r="I43" s="105"/>
-      <c r="J43" s="106"/>
-      <c r="K43" s="107"/>
-      <c r="L43" s="108"/>
-      <c r="M43" s="109"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="101"/>
+      <c r="F43" s="102"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="103"/>
+      <c r="I43" s="104"/>
+      <c r="J43" s="105"/>
+      <c r="K43" s="106"/>
+      <c r="L43" s="107"/>
+      <c r="M43" s="108"/>
     </row>
     <row r="44" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="111"/>
-      <c r="B44" s="112"/>
-      <c r="C44" s="113"/>
-      <c r="D44" s="114"/>
-      <c r="E44" s="115"/>
-      <c r="F44" s="115"/>
-      <c r="G44" s="115"/>
-      <c r="H44" s="116"/>
-      <c r="I44" s="114"/>
-      <c r="J44" s="117"/>
-      <c r="K44" s="117"/>
-      <c r="L44" s="117"/>
-      <c r="M44" s="118"/>
+      <c r="A44" s="109"/>
+      <c r="B44" s="110"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="112"/>
+      <c r="E44" s="113"/>
+      <c r="F44" s="113"/>
+      <c r="G44" s="113"/>
+      <c r="H44" s="114"/>
+      <c r="I44" s="112"/>
+      <c r="J44" s="115"/>
+      <c r="K44" s="115"/>
+      <c r="L44" s="115"/>
+      <c r="M44" s="116"/>
     </row>
     <row r="45" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="119"/>
-      <c r="B45" s="120"/>
-      <c r="C45" s="121"/>
-      <c r="D45" s="122"/>
-      <c r="E45" s="122"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="123"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="114"/>
-      <c r="J45" s="123"/>
-      <c r="K45" s="123"/>
-      <c r="L45" s="123"/>
-      <c r="M45" s="124"/>
+      <c r="A45" s="117"/>
+      <c r="B45" s="118"/>
+      <c r="C45" s="119"/>
+      <c r="D45" s="120"/>
+      <c r="E45" s="120"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="121"/>
+      <c r="H45" s="118"/>
+      <c r="I45" s="112"/>
+      <c r="J45" s="121"/>
+      <c r="K45" s="121"/>
+      <c r="L45" s="121"/>
+      <c r="M45" s="122"/>
     </row>
     <row r="46" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="125" t="s">
+      <c r="A46" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="120"/>
-      <c r="C46" s="123"/>
-      <c r="D46" s="126"/>
-      <c r="E46" s="126"/>
-      <c r="F46" s="123"/>
-      <c r="G46" s="123" t="s">
+      <c r="B46" s="118"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="124"/>
+      <c r="E46" s="124"/>
+      <c r="F46" s="121"/>
+      <c r="G46" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="120"/>
-      <c r="I46" s="120"/>
-      <c r="J46" s="123"/>
-      <c r="K46" s="123"/>
-      <c r="L46" s="123"/>
-      <c r="M46" s="124"/>
+      <c r="H46" s="118"/>
+      <c r="I46" s="118"/>
+      <c r="J46" s="121"/>
+      <c r="K46" s="121"/>
+      <c r="L46" s="121"/>
+      <c r="M46" s="122"/>
     </row>
     <row r="47" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="127"/>
-      <c r="B47" s="128"/>
-      <c r="C47" s="128"/>
-      <c r="D47" s="128"/>
-      <c r="E47" s="128"/>
-      <c r="F47" s="128"/>
-      <c r="G47" s="128"/>
-      <c r="H47" s="128"/>
-      <c r="I47" s="128"/>
-      <c r="J47" s="128"/>
-      <c r="K47" s="128"/>
-      <c r="L47" s="128"/>
-      <c r="M47" s="129"/>
+      <c r="A47" s="125"/>
+      <c r="B47" s="126"/>
+      <c r="C47" s="126"/>
+      <c r="D47" s="126"/>
+      <c r="E47" s="126"/>
+      <c r="F47" s="126"/>
+      <c r="G47" s="126"/>
+      <c r="H47" s="126"/>
+      <c r="I47" s="126"/>
+      <c r="J47" s="126"/>
+      <c r="K47" s="126"/>
+      <c r="L47" s="126"/>
+      <c r="M47" s="127"/>
     </row>
     <row r="48" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="130"/>
-      <c r="B48" s="131"/>
-      <c r="C48" s="131"/>
-      <c r="D48" s="131"/>
-      <c r="E48" s="131"/>
-      <c r="F48" s="131"/>
-      <c r="G48" s="131"/>
-      <c r="H48" s="131"/>
-      <c r="I48" s="131"/>
-      <c r="J48" s="131"/>
-      <c r="K48" s="131"/>
-      <c r="L48" s="131"/>
-      <c r="M48" s="132"/>
+      <c r="A48" s="128"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="129"/>
+      <c r="D48" s="129"/>
+      <c r="E48" s="129"/>
+      <c r="F48" s="129"/>
+      <c r="G48" s="129"/>
+      <c r="H48" s="129"/>
+      <c r="I48" s="129"/>
+      <c r="J48" s="129"/>
+      <c r="K48" s="129"/>
+      <c r="L48" s="129"/>
+      <c r="M48" s="130"/>
     </row>
     <row r="49" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0"/>
@@ -39640,28 +39626,23 @@
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D46:E46"/>
   </mergeCells>
-  <conditionalFormatting sqref="B12:B16,B33:B40,B26:B30,B19:B23">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>OR(#ref!=1,#ref!=7)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>OR(#ref!=1,#ref!=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B25">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>OR(#ref!=1,#ref!=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:B18">
-    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>OR(#ref!=1,#ref!=7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>OR(#ref!=1,#ref!=7)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>